<commit_message>
feat: treasure demon fusion
</commit_message>
<xml_diff>
--- a/compendium.xlsx
+++ b/compendium.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Documents\Persona5R fusion helper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C1EBD6-D83B-4F43-BB23-09873676E68F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A039E6AD-CBD8-4F6B-831F-44A316466EDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1E92B499-8CBF-4ECC-9270-D56049531E95}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="263">
   <si>
     <t>Arcana</t>
   </si>
@@ -795,6 +795,36 @@
   </si>
   <si>
     <t>DLC</t>
+  </si>
+  <si>
+    <t>Crystal Skull</t>
+  </si>
+  <si>
+    <t>Treasure</t>
+  </si>
+  <si>
+    <t>Koh-i-Noor</t>
+  </si>
+  <si>
+    <t>Queen's Necklace</t>
+  </si>
+  <si>
+    <t>Regent</t>
+  </si>
+  <si>
+    <t>Stone of Scone</t>
+  </si>
+  <si>
+    <t>Orlov</t>
+  </si>
+  <si>
+    <t>Emperor's Amulet</t>
+  </si>
+  <si>
+    <t>Hope Diamond</t>
+  </si>
+  <si>
+    <t>Orichalcum</t>
   </si>
 </sst>
 </file>
@@ -1146,15 +1176,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D513931B-8F6D-45F8-BC1F-CF8BDE5CE417}">
-  <dimension ref="A1:E224"/>
+  <dimension ref="A1:F233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
-      <selection activeCell="J213" sqref="J213"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1170,8 +1200,11 @@
       <c r="E1" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1182,7 +1215,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1193,7 +1226,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1207,7 +1240,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1221,7 +1254,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1232,7 +1265,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1246,7 +1279,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1260,7 +1293,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1274,7 +1307,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1288,7 +1321,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1299,7 +1332,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1310,7 +1343,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1324,398 +1357,410 @@
         <v>251</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
       <c r="B14">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+      <c r="F14" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
       <c r="B15">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="D15" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
       <c r="B16">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
       <c r="B17">
+        <v>83</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18">
         <v>95</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>19</v>
       </c>
-      <c r="D17" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18">
-        <v>2</v>
-      </c>
-      <c r="C18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
       <c r="B19">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22">
+        <v>17</v>
+      </c>
+      <c r="C22" t="s">
         <v>24</v>
       </c>
-      <c r="C22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
       <c r="B23">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>20</v>
       </c>
       <c r="B24">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>20</v>
       </c>
       <c r="B25">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>20</v>
       </c>
       <c r="B26">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>20</v>
       </c>
       <c r="B27">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="C27" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>20</v>
       </c>
       <c r="B28">
+        <v>83</v>
+      </c>
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29">
         <v>86</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29">
-        <v>6</v>
-      </c>
-      <c r="C29" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>32</v>
       </c>
       <c r="B30">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>32</v>
       </c>
       <c r="B31">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
       <c r="B32">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C32" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+      <c r="F32" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
       <c r="B33">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="C33" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="B34">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C34" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>32</v>
       </c>
       <c r="B35">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="C35" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>32</v>
       </c>
       <c r="B36">
+        <v>53</v>
+      </c>
+      <c r="C36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37">
+        <v>77</v>
+      </c>
+      <c r="C37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38">
         <v>83</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C38" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>41</v>
-      </c>
-      <c r="B37">
-        <v>20</v>
-      </c>
-      <c r="C37" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>41</v>
-      </c>
-      <c r="B38">
-        <v>26</v>
-      </c>
-      <c r="C38" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>41</v>
       </c>
       <c r="B39">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="C39" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+      <c r="F39" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>41</v>
       </c>
       <c r="B40">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C40" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
       <c r="B41">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="C41" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
       <c r="B42">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="C42" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>41</v>
       </c>
       <c r="B43">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="C43" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>41</v>
       </c>
       <c r="B44">
+        <v>56</v>
+      </c>
+      <c r="C44" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45">
+        <v>63</v>
+      </c>
+      <c r="C45" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>41</v>
+      </c>
+      <c r="B46">
+        <v>81</v>
+      </c>
+      <c r="C46" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47">
         <v>85</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C47" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>50</v>
-      </c>
-      <c r="B45">
-        <v>16</v>
-      </c>
-      <c r="C45" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>50</v>
-      </c>
-      <c r="B46">
-        <v>28</v>
-      </c>
-      <c r="C46" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>50</v>
-      </c>
-      <c r="B47">
-        <v>36</v>
-      </c>
-      <c r="C47" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>50</v>
       </c>
       <c r="B48">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="C48" t="s">
-        <v>54</v>
+        <v>257</v>
+      </c>
+      <c r="F48" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1723,10 +1768,10 @@
         <v>50</v>
       </c>
       <c r="B49">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="C49" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1734,10 +1779,10 @@
         <v>50</v>
       </c>
       <c r="B50">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="C50" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1745,10 +1790,10 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>82</v>
+        <v>36</v>
       </c>
       <c r="C51" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1756,54 +1801,54 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="C52" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B53">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="C53" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B54">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="C54" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B55">
-        <v>25</v>
+        <v>82</v>
       </c>
       <c r="C55" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B56">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="C56" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1811,10 +1856,10 @@
         <v>59</v>
       </c>
       <c r="B57">
-        <v>52</v>
+        <v>9</v>
       </c>
       <c r="C57" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1822,10 +1867,10 @@
         <v>59</v>
       </c>
       <c r="B58">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="C58" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1833,57 +1878,57 @@
         <v>59</v>
       </c>
       <c r="B59">
-        <v>76</v>
+        <v>25</v>
       </c>
       <c r="C59" t="s">
-        <v>66</v>
-      </c>
-      <c r="D59" t="s">
-        <v>251</v>
+        <v>62</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B60">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="C60" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B61">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="C61" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>59</v>
+      </c>
+      <c r="B62">
         <v>67</v>
       </c>
-      <c r="B62">
-        <v>19</v>
-      </c>
       <c r="C62" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B63">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="C63" t="s">
-        <v>71</v>
+        <v>66</v>
+      </c>
+      <c r="D63" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1891,10 +1936,10 @@
         <v>67</v>
       </c>
       <c r="B64">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="C64" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -1902,10 +1947,10 @@
         <v>67</v>
       </c>
       <c r="B65">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="C65" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -1913,10 +1958,10 @@
         <v>67</v>
       </c>
       <c r="B66">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C66" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -1924,10 +1969,10 @@
         <v>67</v>
       </c>
       <c r="B67">
-        <v>78</v>
+        <v>29</v>
       </c>
       <c r="C67" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -1935,54 +1980,54 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>85</v>
+        <v>42</v>
       </c>
       <c r="C68" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B69">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="C69" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B70">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="C70" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B71">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="C71" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B72">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="C72" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -1990,10 +2035,10 @@
         <v>77</v>
       </c>
       <c r="B73">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="C73" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -2001,10 +2046,10 @@
         <v>77</v>
       </c>
       <c r="B74">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="C74" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -2012,13 +2057,10 @@
         <v>77</v>
       </c>
       <c r="B75">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="C75" t="s">
-        <v>84</v>
-      </c>
-      <c r="E75" t="s">
-        <v>251</v>
+        <v>80</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -2026,13 +2068,10 @@
         <v>77</v>
       </c>
       <c r="B76">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="C76" t="s">
-        <v>85</v>
-      </c>
-      <c r="E76" t="s">
-        <v>251</v>
+        <v>81</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2040,10 +2079,10 @@
         <v>77</v>
       </c>
       <c r="B77">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="C77" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -2051,10 +2090,10 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="C78" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -2062,57 +2101,63 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>88</v>
+        <v>46</v>
       </c>
       <c r="C79" t="s">
-        <v>88</v>
-      </c>
-      <c r="D79" t="s">
+        <v>84</v>
+      </c>
+      <c r="E79" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B80">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="C80" t="s">
-        <v>90</v>
+        <v>85</v>
+      </c>
+      <c r="E80" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B81">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="C81" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B82">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="C82" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B83">
-        <v>41</v>
+        <v>88</v>
       </c>
       <c r="C83" t="s">
-        <v>93</v>
+        <v>88</v>
+      </c>
+      <c r="D83" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2120,10 +2165,10 @@
         <v>89</v>
       </c>
       <c r="B84">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="C84" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2131,10 +2176,10 @@
         <v>89</v>
       </c>
       <c r="B85">
-        <v>68</v>
+        <v>14</v>
       </c>
       <c r="C85" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -2142,10 +2187,10 @@
         <v>89</v>
       </c>
       <c r="B86">
-        <v>72</v>
+        <v>29</v>
       </c>
       <c r="C86" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2153,10 +2198,10 @@
         <v>89</v>
       </c>
       <c r="B87">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="C87" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2164,57 +2209,57 @@
         <v>89</v>
       </c>
       <c r="B88">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="C88" t="s">
-        <v>98</v>
-      </c>
-      <c r="D88" t="s">
-        <v>251</v>
+        <v>94</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="B89">
-        <v>4</v>
+        <v>68</v>
       </c>
       <c r="C89" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="B90">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="C90" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="B91">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="C91" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="B92">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="C92" t="s">
-        <v>103</v>
+        <v>98</v>
+      </c>
+      <c r="D92" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -2222,10 +2267,10 @@
         <v>99</v>
       </c>
       <c r="B93">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C93" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -2233,10 +2278,10 @@
         <v>99</v>
       </c>
       <c r="B94">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C94" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -2244,10 +2289,10 @@
         <v>99</v>
       </c>
       <c r="B95">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="C95" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -2255,825 +2300,825 @@
         <v>99</v>
       </c>
       <c r="B96">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="C96" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>99</v>
       </c>
       <c r="B97">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="C97" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>99</v>
       </c>
       <c r="B98">
-        <v>70</v>
+        <v>31</v>
       </c>
       <c r="C98" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>99</v>
       </c>
       <c r="B99">
-        <v>86</v>
+        <v>35</v>
       </c>
       <c r="C99" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>99</v>
       </c>
       <c r="B100">
+        <v>42</v>
+      </c>
+      <c r="C100" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>99</v>
+      </c>
+      <c r="B101">
+        <v>49</v>
+      </c>
+      <c r="C101" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>99</v>
+      </c>
+      <c r="B102">
+        <v>70</v>
+      </c>
+      <c r="C102" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>99</v>
+      </c>
+      <c r="B103">
+        <v>86</v>
+      </c>
+      <c r="C103" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>99</v>
+      </c>
+      <c r="B104">
         <v>89</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C104" t="s">
         <v>111</v>
       </c>
-      <c r="D100" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>112</v>
-      </c>
-      <c r="B101">
-        <v>26</v>
-      </c>
-      <c r="C101" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>112</v>
-      </c>
-      <c r="B102">
-        <v>30</v>
-      </c>
-      <c r="C102" t="s">
-        <v>114</v>
-      </c>
-      <c r="E102" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>112</v>
-      </c>
-      <c r="B103">
-        <v>34</v>
-      </c>
-      <c r="C103" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>112</v>
-      </c>
-      <c r="B104">
-        <v>39</v>
-      </c>
-      <c r="C104" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D104" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>112</v>
       </c>
       <c r="B105">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="C105" t="s">
-        <v>117</v>
-      </c>
-      <c r="E105" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="F105" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>112</v>
       </c>
       <c r="B106">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="C106" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>112</v>
       </c>
       <c r="B107">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="C107" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+      <c r="E107" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>112</v>
       </c>
       <c r="B108">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="C108" t="s">
-        <v>120</v>
-      </c>
-      <c r="E108" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>112</v>
       </c>
       <c r="B109">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="C109" t="s">
-        <v>121</v>
-      </c>
-      <c r="E109" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>112</v>
       </c>
       <c r="B110">
+        <v>42</v>
+      </c>
+      <c r="C110" t="s">
+        <v>117</v>
+      </c>
+      <c r="E110" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>112</v>
+      </c>
+      <c r="B111">
+        <v>46</v>
+      </c>
+      <c r="C111" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>112</v>
+      </c>
+      <c r="B112">
+        <v>52</v>
+      </c>
+      <c r="C112" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>112</v>
+      </c>
+      <c r="B113">
+        <v>56</v>
+      </c>
+      <c r="C113" t="s">
+        <v>120</v>
+      </c>
+      <c r="E113" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>112</v>
+      </c>
+      <c r="B114">
+        <v>62</v>
+      </c>
+      <c r="C114" t="s">
+        <v>121</v>
+      </c>
+      <c r="E114" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>112</v>
+      </c>
+      <c r="B115">
         <v>69</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C115" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>123</v>
-      </c>
-      <c r="B111">
-        <v>6</v>
-      </c>
-      <c r="C111" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>123</v>
-      </c>
-      <c r="B112">
-        <v>15</v>
-      </c>
-      <c r="C112" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>123</v>
-      </c>
-      <c r="B113">
-        <v>20</v>
-      </c>
-      <c r="C113" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>123</v>
-      </c>
-      <c r="B114">
-        <v>24</v>
-      </c>
-      <c r="C114" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>123</v>
-      </c>
-      <c r="B115">
-        <v>31</v>
-      </c>
-      <c r="C115" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>123</v>
       </c>
       <c r="B116">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="C116" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>123</v>
       </c>
       <c r="B117">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="C117" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>123</v>
       </c>
       <c r="B118">
-        <v>74</v>
+        <v>20</v>
       </c>
       <c r="C118" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>123</v>
       </c>
       <c r="B119">
+        <v>24</v>
+      </c>
+      <c r="C119" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>123</v>
+      </c>
+      <c r="B120">
+        <v>30</v>
+      </c>
+      <c r="C120" t="s">
+        <v>259</v>
+      </c>
+      <c r="F120" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>123</v>
+      </c>
+      <c r="B121">
+        <v>31</v>
+      </c>
+      <c r="C121" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>123</v>
+      </c>
+      <c r="B122">
+        <v>44</v>
+      </c>
+      <c r="C122" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>123</v>
+      </c>
+      <c r="B123">
+        <v>64</v>
+      </c>
+      <c r="C123" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>123</v>
+      </c>
+      <c r="B124">
+        <v>74</v>
+      </c>
+      <c r="C124" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>123</v>
+      </c>
+      <c r="B125">
         <v>80</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C125" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>133</v>
-      </c>
-      <c r="B120">
-        <v>9</v>
-      </c>
-      <c r="C120" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>133</v>
-      </c>
-      <c r="B121">
-        <v>14</v>
-      </c>
-      <c r="C121" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>133</v>
-      </c>
-      <c r="B122">
-        <v>21</v>
-      </c>
-      <c r="C122" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>133</v>
-      </c>
-      <c r="B123">
-        <v>26</v>
-      </c>
-      <c r="C123" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>133</v>
-      </c>
-      <c r="B124">
-        <v>42</v>
-      </c>
-      <c r="C124" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>133</v>
-      </c>
-      <c r="B125">
-        <v>51</v>
-      </c>
-      <c r="C125" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>133</v>
       </c>
       <c r="B126">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="C126" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>133</v>
       </c>
       <c r="B127">
-        <v>73</v>
+        <v>14</v>
       </c>
       <c r="C127" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>133</v>
       </c>
       <c r="B128">
+        <v>21</v>
+      </c>
+      <c r="C128" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>133</v>
+      </c>
+      <c r="B129">
+        <v>26</v>
+      </c>
+      <c r="C129" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>133</v>
+      </c>
+      <c r="B130">
+        <v>35</v>
+      </c>
+      <c r="C130" t="s">
+        <v>260</v>
+      </c>
+      <c r="F130" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>133</v>
+      </c>
+      <c r="B131">
+        <v>42</v>
+      </c>
+      <c r="C131" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>133</v>
+      </c>
+      <c r="B132">
+        <v>51</v>
+      </c>
+      <c r="C132" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>133</v>
+      </c>
+      <c r="B133">
+        <v>60</v>
+      </c>
+      <c r="C133" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>133</v>
+      </c>
+      <c r="B134">
+        <v>73</v>
+      </c>
+      <c r="C134" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>133</v>
+      </c>
+      <c r="B135">
         <v>82</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C135" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>143</v>
-      </c>
-      <c r="B129">
-        <v>3</v>
-      </c>
-      <c r="C129" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>143</v>
-      </c>
-      <c r="B130">
-        <v>9</v>
-      </c>
-      <c r="C130" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>143</v>
-      </c>
-      <c r="B131">
-        <v>17</v>
-      </c>
-      <c r="C131" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>143</v>
-      </c>
-      <c r="B132">
-        <v>20</v>
-      </c>
-      <c r="C132" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>143</v>
-      </c>
-      <c r="B133">
-        <v>28</v>
-      </c>
-      <c r="C133" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>143</v>
-      </c>
-      <c r="B134">
-        <v>37</v>
-      </c>
-      <c r="C134" t="s">
-        <v>149</v>
-      </c>
-      <c r="D134" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>143</v>
-      </c>
-      <c r="B135">
-        <v>54</v>
-      </c>
-      <c r="C135" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>143</v>
       </c>
       <c r="B136">
-        <v>62</v>
+        <v>3</v>
       </c>
       <c r="C136" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>143</v>
       </c>
       <c r="B137">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="C137" t="s">
-        <v>152</v>
-      </c>
-      <c r="E137" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>143</v>
       </c>
       <c r="B138">
-        <v>69</v>
+        <v>17</v>
       </c>
       <c r="C138" t="s">
-        <v>153</v>
-      </c>
-      <c r="E138" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>143</v>
       </c>
       <c r="B139">
-        <v>72</v>
+        <v>20</v>
       </c>
       <c r="C139" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>143</v>
       </c>
       <c r="B140">
+        <v>28</v>
+      </c>
+      <c r="C140" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>143</v>
+      </c>
+      <c r="B141">
+        <v>37</v>
+      </c>
+      <c r="C141" t="s">
+        <v>149</v>
+      </c>
+      <c r="D141" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>143</v>
+      </c>
+      <c r="B142">
+        <v>40</v>
+      </c>
+      <c r="C142" t="s">
+        <v>261</v>
+      </c>
+      <c r="F142" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>143</v>
+      </c>
+      <c r="B143">
+        <v>54</v>
+      </c>
+      <c r="C143" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>143</v>
+      </c>
+      <c r="B144">
+        <v>62</v>
+      </c>
+      <c r="C144" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>143</v>
+      </c>
+      <c r="B145">
+        <v>65</v>
+      </c>
+      <c r="C145" t="s">
+        <v>152</v>
+      </c>
+      <c r="E145" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>143</v>
+      </c>
+      <c r="B146">
+        <v>69</v>
+      </c>
+      <c r="C146" t="s">
+        <v>153</v>
+      </c>
+      <c r="E146" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>143</v>
+      </c>
+      <c r="B147">
+        <v>72</v>
+      </c>
+      <c r="C147" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>143</v>
+      </c>
+      <c r="B148">
         <v>83</v>
       </c>
-      <c r="C140" t="s">
+      <c r="C148" t="s">
         <v>155</v>
       </c>
-      <c r="D140" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>156</v>
-      </c>
-      <c r="B141">
-        <v>7</v>
-      </c>
-      <c r="C141" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>156</v>
-      </c>
-      <c r="B142">
-        <v>11</v>
-      </c>
-      <c r="C142" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>156</v>
-      </c>
-      <c r="B143">
-        <v>15</v>
-      </c>
-      <c r="C143" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>156</v>
-      </c>
-      <c r="B144">
-        <v>22</v>
-      </c>
-      <c r="C144" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>156</v>
-      </c>
-      <c r="B145">
-        <v>33</v>
-      </c>
-      <c r="C145" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>156</v>
-      </c>
-      <c r="B146">
-        <v>45</v>
-      </c>
-      <c r="C146" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>156</v>
-      </c>
-      <c r="B147">
-        <v>55</v>
-      </c>
-      <c r="C147" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>156</v>
-      </c>
-      <c r="B148">
-        <v>77</v>
-      </c>
-      <c r="C148" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D148" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>156</v>
       </c>
       <c r="B149">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="C149" t="s">
-        <v>165</v>
-      </c>
-      <c r="D149" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B150">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C150" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B151">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C151" t="s">
-        <v>168</v>
-      </c>
-      <c r="D151" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B152">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C152" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B153">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C153" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B154">
         <v>45</v>
       </c>
       <c r="C154" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B155">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C155" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B156">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C156" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B157">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C157" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+      <c r="D157" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>166</v>
       </c>
       <c r="B158">
-        <v>87</v>
+        <v>5</v>
       </c>
       <c r="C158" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="B159">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C159" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+      <c r="D159" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="B160">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="C160" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="B161">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C161" t="s">
-        <v>179</v>
-      </c>
-      <c r="E161" t="s">
-        <v>251</v>
+        <v>170</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="B162">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C162" t="s">
-        <v>180</v>
-      </c>
-      <c r="E162" t="s">
-        <v>251</v>
+        <v>171</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="B163">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C163" t="s">
-        <v>181</v>
-      </c>
-      <c r="D163" t="s">
-        <v>251</v>
+        <v>172</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="B164">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="C164" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="B165">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="C165" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="B166">
         <v>87</v>
       </c>
       <c r="C166" t="s">
-        <v>184</v>
-      </c>
-      <c r="D166" t="s">
-        <v>251</v>
+        <v>175</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -3081,93 +3126,96 @@
         <v>176</v>
       </c>
       <c r="B167">
-        <v>90</v>
+        <v>37</v>
       </c>
       <c r="C167" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B168">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="C168" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B169">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="C169" t="s">
-        <v>188</v>
+        <v>179</v>
+      </c>
+      <c r="E169" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B170">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="C170" t="s">
-        <v>189</v>
-      </c>
-      <c r="D170" t="s">
+        <v>180</v>
+      </c>
+      <c r="E170" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B171">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="C171" t="s">
-        <v>190</v>
+        <v>181</v>
+      </c>
+      <c r="D171" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B172">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C172" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B173">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C173" t="s">
-        <v>192</v>
-      </c>
-      <c r="D173" t="s">
-        <v>251</v>
+        <v>183</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B174">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="C174" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D174" t="s">
         <v>251</v>
@@ -3175,13 +3223,13 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B175">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C175" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
@@ -3189,107 +3237,110 @@
         <v>186</v>
       </c>
       <c r="B176">
-        <v>93</v>
+        <v>11</v>
       </c>
       <c r="C176" t="s">
-        <v>195</v>
-      </c>
-      <c r="D176" t="s">
-        <v>251</v>
+        <v>187</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="B177">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C177" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="B178">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="C178" t="s">
-        <v>198</v>
+        <v>189</v>
+      </c>
+      <c r="D178" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="B179">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="C179" t="s">
-        <v>199</v>
-      </c>
-      <c r="E179" t="s">
-        <v>251</v>
+        <v>190</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="B180">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="C180" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="B181">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="C181" t="s">
-        <v>201</v>
+        <v>192</v>
+      </c>
+      <c r="D181" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="B182">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="C182" t="s">
-        <v>202</v>
-      </c>
-      <c r="E182" t="s">
+        <v>193</v>
+      </c>
+      <c r="D182" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="B183">
-        <v>33</v>
+        <v>84</v>
       </c>
       <c r="C183" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="B184">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="C184" t="s">
-        <v>204</v>
+        <v>195</v>
+      </c>
+      <c r="D184" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
@@ -3297,13 +3348,10 @@
         <v>196</v>
       </c>
       <c r="B185">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="C185" t="s">
-        <v>205</v>
-      </c>
-      <c r="E185" t="s">
-        <v>251</v>
+        <v>197</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
@@ -3311,13 +3359,10 @@
         <v>196</v>
       </c>
       <c r="B186">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="C186" t="s">
-        <v>206</v>
-      </c>
-      <c r="E186" t="s">
-        <v>251</v>
+        <v>198</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
@@ -3325,10 +3370,13 @@
         <v>196</v>
       </c>
       <c r="B187">
-        <v>60</v>
+        <v>16</v>
       </c>
       <c r="C187" t="s">
-        <v>207</v>
+        <v>199</v>
+      </c>
+      <c r="E187" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
@@ -3336,10 +3384,10 @@
         <v>196</v>
       </c>
       <c r="B188">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="C188" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
@@ -3347,203 +3395,197 @@
         <v>196</v>
       </c>
       <c r="B189">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="C189" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="B190">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C190" t="s">
-        <v>211</v>
+        <v>202</v>
+      </c>
+      <c r="E190" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="B191">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C191" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="B192">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C192" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="B193">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C193" t="s">
-        <v>214</v>
+        <v>205</v>
+      </c>
+      <c r="E193" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="B194">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C194" t="s">
-        <v>215</v>
+        <v>206</v>
+      </c>
+      <c r="E194" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="B195">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C195" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="B196">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C196" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="B197">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C197" t="s">
-        <v>218</v>
-      </c>
-      <c r="D197" t="s">
-        <v>251</v>
+        <v>209</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="B198">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="C198" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="B199">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="C199" t="s">
-        <v>221</v>
-      </c>
-      <c r="D199" t="s">
-        <v>251</v>
+        <v>212</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="B200">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="C200" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="B201">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="C201" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="B202">
-        <v>81</v>
+        <v>47</v>
       </c>
       <c r="C202" t="s">
-        <v>224</v>
-      </c>
-      <c r="E202" t="s">
-        <v>251</v>
+        <v>215</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="B203">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="C203" t="s">
-        <v>225</v>
-      </c>
-      <c r="D203" t="s">
-        <v>251</v>
+        <v>216</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="B204">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="C204" t="s">
-        <v>226</v>
-      </c>
-      <c r="D204" t="s">
-        <v>251</v>
+        <v>217</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="B205">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="C205" t="s">
-        <v>227</v>
-      </c>
-      <c r="E205" t="s">
+        <v>218</v>
+      </c>
+      <c r="D205" t="s">
         <v>251</v>
       </c>
     </row>
@@ -3552,222 +3594,339 @@
         <v>219</v>
       </c>
       <c r="B206">
-        <v>92</v>
+        <v>34</v>
       </c>
       <c r="C206" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="B207">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="C207" t="s">
-        <v>230</v>
+        <v>221</v>
+      </c>
+      <c r="D207" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
+        <v>219</v>
+      </c>
+      <c r="B208">
+        <v>64</v>
+      </c>
+      <c r="C208" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>219</v>
+      </c>
+      <c r="B209">
+        <v>75</v>
+      </c>
+      <c r="C209" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>219</v>
+      </c>
+      <c r="B210">
+        <v>81</v>
+      </c>
+      <c r="C210" t="s">
+        <v>224</v>
+      </c>
+      <c r="E210" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>219</v>
+      </c>
+      <c r="B211">
+        <v>82</v>
+      </c>
+      <c r="C211" t="s">
+        <v>225</v>
+      </c>
+      <c r="D211" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>219</v>
+      </c>
+      <c r="B212">
+        <v>87</v>
+      </c>
+      <c r="C212" t="s">
+        <v>226</v>
+      </c>
+      <c r="D212" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>219</v>
+      </c>
+      <c r="B213">
+        <v>90</v>
+      </c>
+      <c r="C213" t="s">
+        <v>227</v>
+      </c>
+      <c r="E213" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>219</v>
+      </c>
+      <c r="B214">
+        <v>92</v>
+      </c>
+      <c r="C214" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
         <v>229</v>
       </c>
-      <c r="B208">
+      <c r="B215">
+        <v>21</v>
+      </c>
+      <c r="C215" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>229</v>
+      </c>
+      <c r="B216">
         <v>27</v>
       </c>
-      <c r="C208" t="s">
+      <c r="C216" t="s">
         <v>231</v>
       </c>
-      <c r="D208" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A209" t="s">
+      <c r="D216" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
         <v>229</v>
       </c>
-      <c r="B209">
+      <c r="B217">
         <v>39</v>
       </c>
-      <c r="C209" t="s">
+      <c r="C217" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A210" t="s">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
         <v>229</v>
       </c>
-      <c r="B210">
+      <c r="B218">
         <v>54</v>
       </c>
-      <c r="C210" t="s">
+      <c r="C218" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
         <v>229</v>
       </c>
-      <c r="B211">
+      <c r="B219">
+        <v>60</v>
+      </c>
+      <c r="C219" t="s">
+        <v>262</v>
+      </c>
+      <c r="F219" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>229</v>
+      </c>
+      <c r="B220">
         <v>65</v>
       </c>
-      <c r="C211" t="s">
+      <c r="C220" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A212" t="s">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
         <v>229</v>
       </c>
-      <c r="B212">
+      <c r="B221">
         <v>76</v>
       </c>
-      <c r="C212" t="s">
+      <c r="C221" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A213" t="s">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
         <v>229</v>
       </c>
-      <c r="B213">
+      <c r="B222">
         <v>84</v>
       </c>
-      <c r="C213" t="s">
+      <c r="C222" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A214" t="s">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
         <v>229</v>
       </c>
-      <c r="B214">
+      <c r="B223">
         <v>93</v>
       </c>
-      <c r="C214" t="s">
+      <c r="C223" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A215" t="s">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
         <v>238</v>
       </c>
-      <c r="B215">
+      <c r="B224">
         <v>12</v>
       </c>
-      <c r="C215" t="s">
+      <c r="C224" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A216" t="s">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
         <v>238</v>
       </c>
-      <c r="B216">
+      <c r="B225">
         <v>22</v>
       </c>
-      <c r="C216" t="s">
+      <c r="C225" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A217" t="s">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
         <v>238</v>
       </c>
-      <c r="B217">
+      <c r="B226">
         <v>32</v>
       </c>
-      <c r="C217" t="s">
+      <c r="C226" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A218" t="s">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
         <v>238</v>
       </c>
-      <c r="B218">
+      <c r="B227">
         <v>44</v>
       </c>
-      <c r="C218" t="s">
+      <c r="C227" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A219" t="s">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
         <v>238</v>
       </c>
-      <c r="B219">
+      <c r="B228">
         <v>57</v>
       </c>
-      <c r="C219" t="s">
+      <c r="C228" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A220" t="s">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
         <v>238</v>
       </c>
-      <c r="B220">
+      <c r="B229">
         <v>62</v>
       </c>
-      <c r="C220" t="s">
+      <c r="C229" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A221" t="s">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
         <v>238</v>
       </c>
-      <c r="B221">
+      <c r="B230">
         <v>71</v>
       </c>
-      <c r="C221" t="s">
+      <c r="C230" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A222" t="s">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
         <v>238</v>
       </c>
-      <c r="B222">
+      <c r="B231">
         <v>80</v>
       </c>
-      <c r="C222" t="s">
+      <c r="C231" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A223" t="s">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
         <v>247</v>
       </c>
-      <c r="B223">
+      <c r="B232">
         <v>80</v>
       </c>
-      <c r="C223" t="s">
+      <c r="C232" t="s">
         <v>248</v>
       </c>
-      <c r="D223" t="s">
-        <v>251</v>
-      </c>
-      <c r="E223" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A224" t="s">
+      <c r="D232" t="s">
+        <v>251</v>
+      </c>
+      <c r="E232" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
         <v>247</v>
       </c>
-      <c r="B224">
+      <c r="B233">
         <v>89</v>
       </c>
-      <c r="C224" t="s">
+      <c r="C233" t="s">
         <v>249</v>
       </c>
-      <c r="D224" t="s">
-        <v>251</v>
-      </c>
-      <c r="E224" t="s">
+      <c r="D233" t="s">
+        <v>251</v>
+      </c>
+      <c r="E233" t="s">
         <v>251</v>
       </c>
     </row>

</xml_diff>